<commit_message>
Update Solution Worksheet Document
</commit_message>
<xml_diff>
--- a/RedwoodPLG/BISolutionWorksheets.xlsx
+++ b/RedwoodPLG/BISolutionWorksheets.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f659aa45aa830916/Fourth Year/Fall Quarter/INFO 3300/Peer Learning Group Project/Redwood-Peer-Learning-Project/RedwoodPLG/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="16" documentId="352216AD6DD537773E45C28CF7384E38FEB306FA" xr6:coauthVersionLast="21" xr6:coauthVersionMax="21" xr10:uidLastSave="{4059203E-B669-4EDD-A3E0-9631B361B072}"/>
+  <xr:revisionPtr revIDLastSave="108" documentId="352216AD6DD537773E45C28CF7384E38FEB306FA" xr6:coauthVersionLast="21" xr6:coauthVersionMax="21" xr10:uidLastSave="{8C7168EC-4E4A-47F4-AB12-BBA0FA22377C}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16538" windowHeight="4575" activeTab="1" xr2:uid="{CF73424B-00BD-4AE5-B259-C98A10007E36}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="105">
   <si>
     <t>Team Member</t>
   </si>
@@ -169,10 +169,178 @@
     <t>Generated</t>
   </si>
   <si>
-    <t>DWRedwoodRealty.dbo.DimListing.ListDate</t>
-  </si>
-  <si>
     <t>DWRedwoodRealty.dbo.DimListing.ListingKey</t>
+  </si>
+  <si>
+    <t>DWRedwoodRealty.dbo.DimAgent</t>
+  </si>
+  <si>
+    <t>Redwood.dbo.Agent</t>
+  </si>
+  <si>
+    <t>DWRedwoodRealty.dbo.DimAgentKey</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>INT</t>
+  </si>
+  <si>
+    <t>DWRedwoodRealty.dbo.DimAgent.FirstName</t>
+  </si>
+  <si>
+    <t>Redwood.dbo.Agent.FirstName</t>
+  </si>
+  <si>
+    <t>Nvarchar(30)</t>
+  </si>
+  <si>
+    <t>Nvarchar(25)</t>
+  </si>
+  <si>
+    <t>DWRedwoodRealty.dbo.DimAgent.LastName</t>
+  </si>
+  <si>
+    <t>Redwood.dbo.Agent.LastName</t>
+  </si>
+  <si>
+    <t>Nvarchar(300)</t>
+  </si>
+  <si>
+    <t>Nvarchar(40)</t>
+  </si>
+  <si>
+    <t>DWRedwoodRealty.dbo.DimAgent.HireDate</t>
+  </si>
+  <si>
+    <t>DateTime</t>
+  </si>
+  <si>
+    <t>DWRedwoodRealty.dbo.DimAgent.DOB</t>
+  </si>
+  <si>
+    <t>DWRedwoodRealty.dbo.DimAgent.LicenseDate</t>
+  </si>
+  <si>
+    <t>DWRedwoodRealty.dbo.DimAgent.Gender</t>
+  </si>
+  <si>
+    <t>Nchar(1)</t>
+  </si>
+  <si>
+    <t>DWRedwoodRealty.dbo.DimContactReason</t>
+  </si>
+  <si>
+    <t>Redwood.dbo.ContactReason</t>
+  </si>
+  <si>
+    <t>DWRedwoodRealty.dbo.DimContactReason.ContactKey</t>
+  </si>
+  <si>
+    <t>DWRedwoodRealty.dbo.DimContactReason.ContactReason</t>
+  </si>
+  <si>
+    <t>Redwood.dbo.ContactReason.ContactReason</t>
+  </si>
+  <si>
+    <t>Nvarchar(15)</t>
+  </si>
+  <si>
+    <t>DWRedwoodRealty.dbo.SalesStatus</t>
+  </si>
+  <si>
+    <t>Redwood.dbo.SalesStatus</t>
+  </si>
+  <si>
+    <t>DWRedwoodRealty.dbo.SalesStatus.StatusKey</t>
+  </si>
+  <si>
+    <t>DWRedwoodRealty.dbo.SalesStatus.SalesStatus</t>
+  </si>
+  <si>
+    <t>Redwood.dbo.SalesStatus.SalesStatus</t>
+  </si>
+  <si>
+    <t>Nvarchar(10)</t>
+  </si>
+  <si>
+    <t>DWRedwoodRealty.dbo.DimListing.BeginListDate</t>
+  </si>
+  <si>
+    <t>Redwood.dbo.Listing.BeginListDate</t>
+  </si>
+  <si>
+    <t>DWRedwoodRealty.dbo.DimListing.EndListDate</t>
+  </si>
+  <si>
+    <t>Redwood.dbo.Listing.EndListDate</t>
+  </si>
+  <si>
+    <t>DWRedwoodRealty.dbo.DimListing.AskingPrice</t>
+  </si>
+  <si>
+    <t>Redwood.dbo.Listing.AskingPrice</t>
+  </si>
+  <si>
+    <t>Money</t>
+  </si>
+  <si>
+    <t>DWRedwoodRealty.dbo.DimProperty</t>
+  </si>
+  <si>
+    <t>Redwood.dbo.Property</t>
+  </si>
+  <si>
+    <t>DWRedwoodRealty.dbo.dimProperty.PropertyKey</t>
+  </si>
+  <si>
+    <t>DWRedwoodRealty.dbo.DimProperty.City</t>
+  </si>
+  <si>
+    <t>Redwood.dbo.Property.City</t>
+  </si>
+  <si>
+    <t>DWRedwoodRealty.dbo.DimProperty.State</t>
+  </si>
+  <si>
+    <t>DWRedwoodRealty.dbo.DimProperty.ZipCode</t>
+  </si>
+  <si>
+    <t>DWRedwoodRealty.dbo.DimProperty.Bedrooms</t>
+  </si>
+  <si>
+    <t>DWRedwoodRealty.dbo.DimProperty.Bathrooms</t>
+  </si>
+  <si>
+    <t>DWRedwoodRealty.dbo.DimProperty.SquareFoot</t>
+  </si>
+  <si>
+    <t>DWRedwoodRealty.dbo.DimProperty.YearBuilt</t>
+  </si>
+  <si>
+    <t>Redwood.dbo.Property.State</t>
+  </si>
+  <si>
+    <t>Redwood.dbo.Property.ZipCode</t>
+  </si>
+  <si>
+    <t>Redwood.dbo.Property.Bedrooms</t>
+  </si>
+  <si>
+    <t>Redwood.dbo.Property.Bathrooms</t>
+  </si>
+  <si>
+    <t>Redwood.dbo.Property.SquareFoot</t>
+  </si>
+  <si>
+    <t>Redwood.dbo.Property.YearBuilt</t>
+  </si>
+  <si>
+    <t>Nvarchar(20)</t>
+  </si>
+  <si>
+    <t>NUMERIC(4)</t>
   </si>
 </sst>
 </file>
@@ -196,7 +364,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -206,6 +374,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -222,12 +396,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -278,8 +453,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{45A67816-CAA5-4C9B-B9BD-DD818D06DF8C}" name="Table3" displayName="Table3" ref="A3:E34" totalsRowShown="0">
-  <autoFilter ref="A3:E34" xr:uid="{37E33246-CBF2-44C3-98B8-75AB4FA424DA}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{45A67816-CAA5-4C9B-B9BD-DD818D06DF8C}" name="Table3" displayName="Table3" ref="A3:E42" totalsRowShown="0">
+  <autoFilter ref="A3:E42" xr:uid="{37E33246-CBF2-44C3-98B8-75AB4FA424DA}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{5711C450-759C-4DA2-B975-CF23F68F15B1}" name="Object Name"/>
     <tableColumn id="2" xr3:uid="{7B1E178C-295E-42C6-9047-ADB8B93DFACF}" name="Description"/>
@@ -668,17 +843,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{538236FA-53CC-471C-8DFB-D0C800A7188D}">
-  <dimension ref="A2:E17"/>
+  <dimension ref="A2:E42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="E42" sqref="E42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="39.86328125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.9296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="53.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.06640625" customWidth="1"/>
     <col min="5" max="5" width="15.86328125" customWidth="1"/>
   </cols>
@@ -905,7 +1080,7 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B16" t="s">
         <v>45</v>
@@ -920,9 +1095,450 @@
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
-        <v>47</v>
+        <v>79</v>
+      </c>
+      <c r="B17" t="s">
+        <v>28</v>
+      </c>
+      <c r="C17" t="s">
+        <v>80</v>
+      </c>
+      <c r="D17" t="s">
+        <v>62</v>
+      </c>
+      <c r="E17" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A18" t="s">
+        <v>81</v>
+      </c>
+      <c r="B18" t="s">
+        <v>28</v>
+      </c>
+      <c r="C18" t="s">
+        <v>82</v>
+      </c>
+      <c r="D18" t="s">
+        <v>62</v>
+      </c>
+      <c r="E18" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A19" t="s">
+        <v>83</v>
+      </c>
+      <c r="B19" t="s">
+        <v>28</v>
+      </c>
+      <c r="C19" t="s">
+        <v>84</v>
+      </c>
+      <c r="D19" t="s">
+        <v>85</v>
+      </c>
+      <c r="E19" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A20" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A21" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A22" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A23" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A24" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C24" s="5" t="str">
+        <f>CONCATENATE("Redwood.dbo.Agent.",RIGHT(A24,(LEN(A24)-(LEN($A$1)+1))))</f>
+        <v>Redwood.dbo.Agent.WRedwoodRealty.dbo.DimAgent.HireDate</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="E24" s="5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A25" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C25" s="5" t="str">
+        <f t="shared" ref="C25:C27" si="0">CONCATENATE("Redwood.dbo.Agent.",RIGHT(A25,(LEN(A25)-(LEN($A$1)+1))))</f>
+        <v>Redwood.dbo.Agent.WRedwoodRealty.dbo.DimAgent.DOB</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="E25" s="5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A26" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C26" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>Redwood.dbo.Agent.WRedwoodRealty.dbo.DimAgent.LicenseDate</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="E26" s="5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A27" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C27" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>Redwood.dbo.Agent.WRedwoodRealty.dbo.DimAgent.Gender</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="E27" s="5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A28" t="s">
+        <v>67</v>
+      </c>
+      <c r="B28" t="s">
+        <v>42</v>
+      </c>
+      <c r="C28" t="s">
+        <v>68</v>
+      </c>
+      <c r="D28" t="s">
+        <v>44</v>
+      </c>
+      <c r="E28" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A29" t="s">
+        <v>69</v>
+      </c>
+      <c r="B29" t="s">
+        <v>45</v>
+      </c>
+      <c r="C29" t="s">
+        <v>46</v>
+      </c>
+      <c r="D29" t="s">
+        <v>51</v>
+      </c>
+      <c r="E29" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A30" t="s">
+        <v>70</v>
+      </c>
+      <c r="B30" t="s">
+        <v>28</v>
+      </c>
+      <c r="C30" t="s">
+        <v>71</v>
+      </c>
+      <c r="D30" t="s">
+        <v>72</v>
+      </c>
+      <c r="E30" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A31" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="D31" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="E31" s="5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A32" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D32" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="E32" s="5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A33" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="D33" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="E33" s="5" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A34" t="s">
+        <v>86</v>
+      </c>
+      <c r="B34" t="s">
+        <v>42</v>
+      </c>
+      <c r="C34" t="s">
+        <v>87</v>
+      </c>
+      <c r="D34" t="s">
+        <v>44</v>
+      </c>
+      <c r="E34" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A35" t="s">
+        <v>88</v>
+      </c>
+      <c r="B35" t="s">
+        <v>45</v>
+      </c>
+      <c r="C35" t="s">
+        <v>46</v>
+      </c>
+      <c r="D35" t="s">
+        <v>29</v>
+      </c>
+      <c r="E35" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A36" t="s">
+        <v>89</v>
+      </c>
+      <c r="B36" t="s">
+        <v>28</v>
+      </c>
+      <c r="C36" t="s">
+        <v>90</v>
+      </c>
+      <c r="D36" t="s">
+        <v>55</v>
+      </c>
+      <c r="E36" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A37" t="s">
+        <v>91</v>
+      </c>
+      <c r="B37" t="s">
+        <v>28</v>
+      </c>
+      <c r="C37" t="s">
+        <v>97</v>
+      </c>
+      <c r="D37" t="s">
+        <v>103</v>
+      </c>
+      <c r="E37" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A38" t="s">
+        <v>92</v>
+      </c>
+      <c r="B38" t="s">
+        <v>28</v>
+      </c>
+      <c r="C38" t="s">
+        <v>98</v>
+      </c>
+      <c r="D38" t="s">
+        <v>103</v>
+      </c>
+      <c r="E38" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A39" t="s">
+        <v>93</v>
+      </c>
+      <c r="B39" t="s">
+        <v>28</v>
+      </c>
+      <c r="C39" t="s">
+        <v>99</v>
+      </c>
+      <c r="D39" t="s">
+        <v>52</v>
+      </c>
+      <c r="E39" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A40" t="s">
+        <v>94</v>
+      </c>
+      <c r="B40" t="s">
+        <v>28</v>
+      </c>
+      <c r="C40" t="s">
+        <v>100</v>
+      </c>
+      <c r="D40" t="s">
+        <v>52</v>
+      </c>
+      <c r="E40" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A41" t="s">
+        <v>95</v>
+      </c>
+      <c r="B41" t="s">
+        <v>28</v>
+      </c>
+      <c r="C41" t="s">
+        <v>101</v>
+      </c>
+      <c r="D41" t="s">
+        <v>52</v>
+      </c>
+      <c r="E41" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A42" t="s">
+        <v>96</v>
+      </c>
+      <c r="B42" t="s">
+        <v>28</v>
+      </c>
+      <c r="C42" t="s">
+        <v>102</v>
+      </c>
+      <c r="D42" t="s">
+        <v>104</v>
+      </c>
+      <c r="E42" t="s">
+        <v>104</v>
       </c>
     </row>
   </sheetData>

</xml_diff>